<commit_message>
Data_cleaning. Limpiando main. Creando función clean_nan_list
</commit_message>
<xml_diff>
--- a/data/output/rs_analysis.xlsx
+++ b/data/output/rs_analysis.xlsx
@@ -6841,16 +6841,16 @@
         <v>45049</v>
       </c>
       <c r="B322">
-        <v>116.98</v>
+        <v>116.711</v>
       </c>
       <c r="C322">
-        <v>105.092</v>
+        <v>104.85</v>
       </c>
       <c r="D322">
-        <v>150.511</v>
+        <v>150.164</v>
       </c>
       <c r="E322">
-        <v>122.321</v>
+        <v>122.039</v>
       </c>
       <c r="F322">
         <v>100</v>
@@ -10921,16 +10921,16 @@
         <v>45363</v>
       </c>
       <c r="B526">
-        <v>119.433</v>
+        <v>120.118</v>
       </c>
       <c r="C526">
-        <v>134.435</v>
+        <v>135.206</v>
       </c>
       <c r="D526">
-        <v>158.613</v>
+        <v>159.522</v>
       </c>
       <c r="E526">
-        <v>142.497</v>
+        <v>143.314</v>
       </c>
       <c r="F526">
         <v>100</v>
@@ -10944,10 +10944,10 @@
         <v>120.584</v>
       </c>
       <c r="C527">
-        <v>135.394</v>
+        <v>135.395</v>
       </c>
       <c r="D527">
-        <v>157.967</v>
+        <v>157.968</v>
       </c>
       <c r="E527">
         <v>139.031</v>
@@ -10961,10 +10961,10 @@
         <v>45365</v>
       </c>
       <c r="B528">
-        <v>120.011</v>
+        <v>120.012</v>
       </c>
       <c r="C528">
-        <v>134.322</v>
+        <v>134.323</v>
       </c>
       <c r="D528">
         <v>158.05</v>
@@ -10984,7 +10984,7 @@
         <v>120.12</v>
       </c>
       <c r="C529">
-        <v>136.184</v>
+        <v>136.185</v>
       </c>
       <c r="D529">
         <v>159.307</v>
@@ -11001,16 +11001,16 @@
         <v>45369</v>
       </c>
       <c r="B530">
-        <v>120.047</v>
+        <v>120.501</v>
       </c>
       <c r="C530">
-        <v>137.796</v>
+        <v>138.317</v>
       </c>
       <c r="D530">
-        <v>162.031</v>
+        <v>162.644</v>
       </c>
       <c r="E530">
-        <v>143.209</v>
+        <v>143.75</v>
       </c>
       <c r="F530">
         <v>100</v>
@@ -11024,13 +11024,13 @@
         <v>123.137</v>
       </c>
       <c r="C531">
-        <v>137.077</v>
+        <v>137.078</v>
       </c>
       <c r="D531">
-        <v>161.548</v>
+        <v>161.549</v>
       </c>
       <c r="E531">
-        <v>143.689</v>
+        <v>143.69</v>
       </c>
       <c r="F531">
         <v>100</v>
@@ -11044,13 +11044,13 @@
         <v>124.791</v>
       </c>
       <c r="C532">
-        <v>138.961</v>
+        <v>138.962</v>
       </c>
       <c r="D532">
-        <v>162.443</v>
+        <v>162.444</v>
       </c>
       <c r="E532">
-        <v>146.697</v>
+        <v>146.698</v>
       </c>
       <c r="F532">
         <v>100</v>
@@ -11064,10 +11064,10 @@
         <v>126.627</v>
       </c>
       <c r="C533">
-        <v>139.752</v>
+        <v>139.753</v>
       </c>
       <c r="D533">
-        <v>164.279</v>
+        <v>164.28</v>
       </c>
       <c r="E533">
         <v>145.734</v>
@@ -11081,16 +11081,16 @@
         <v>45373</v>
       </c>
       <c r="B534">
-        <v>126.212</v>
+        <v>126.213</v>
       </c>
       <c r="C534">
         <v>140.426</v>
       </c>
       <c r="D534">
-        <v>164.699</v>
+        <v>164.7</v>
       </c>
       <c r="E534">
-        <v>147.533</v>
+        <v>147.534</v>
       </c>
       <c r="F534">
         <v>100</v>
@@ -11107,10 +11107,10 @@
         <v>140.223</v>
       </c>
       <c r="D535">
-        <v>164.478</v>
+        <v>164.479</v>
       </c>
       <c r="E535">
-        <v>146.331</v>
+        <v>146.332</v>
       </c>
       <c r="F535">
         <v>100</v>
@@ -11124,7 +11124,7 @@
         <v>126.712</v>
       </c>
       <c r="C536">
-        <v>140.1</v>
+        <v>140.101</v>
       </c>
       <c r="D536">
         <v>164.09</v>
@@ -11144,13 +11144,13 @@
         <v>125.585</v>
       </c>
       <c r="C537">
-        <v>140.674</v>
+        <v>140.675</v>
       </c>
       <c r="D537">
         <v>164.995</v>
       </c>
       <c r="E537">
-        <v>146.695</v>
+        <v>146.696</v>
       </c>
       <c r="F537">
         <v>100</v>
@@ -11161,13 +11161,13 @@
         <v>45385</v>
       </c>
       <c r="B538">
-        <v>123.55</v>
+        <v>123.551</v>
       </c>
       <c r="C538">
         <v>140.656</v>
       </c>
       <c r="D538">
-        <v>165.844</v>
+        <v>165.845</v>
       </c>
       <c r="E538">
         <v>148.207</v>
@@ -11204,13 +11204,13 @@
         <v>122.718</v>
       </c>
       <c r="C540">
-        <v>142.642</v>
+        <v>142.643</v>
       </c>
       <c r="D540">
-        <v>166.946</v>
+        <v>166.947</v>
       </c>
       <c r="E540">
-        <v>149.522</v>
+        <v>149.523</v>
       </c>
       <c r="F540">
         <v>100</v>
@@ -11221,16 +11221,16 @@
         <v>45390</v>
       </c>
       <c r="B541">
-        <v>124.379</v>
+        <v>124.38</v>
       </c>
       <c r="C541">
-        <v>142.88</v>
+        <v>142.881</v>
       </c>
       <c r="D541">
         <v>167.715</v>
       </c>
       <c r="E541">
-        <v>149.445</v>
+        <v>149.446</v>
       </c>
       <c r="F541">
         <v>100</v>
@@ -11241,16 +11241,16 @@
         <v>45391</v>
       </c>
       <c r="B542">
-        <v>126.003</v>
+        <v>126.004</v>
       </c>
       <c r="C542">
-        <v>143.245</v>
+        <v>143.246</v>
       </c>
       <c r="D542">
-        <v>166.971</v>
+        <v>166.972</v>
       </c>
       <c r="E542">
-        <v>148.224</v>
+        <v>148.225</v>
       </c>
       <c r="F542">
         <v>100</v>
@@ -11261,13 +11261,13 @@
         <v>45392</v>
       </c>
       <c r="B543">
-        <v>124.654</v>
+        <v>124.655</v>
       </c>
       <c r="C543">
-        <v>143.774</v>
+        <v>143.775</v>
       </c>
       <c r="D543">
-        <v>166.663</v>
+        <v>166.664</v>
       </c>
       <c r="E543">
         <v>146.991</v>
@@ -11281,13 +11281,13 @@
         <v>45393</v>
       </c>
       <c r="B544">
-        <v>124.923</v>
+        <v>124.924</v>
       </c>
       <c r="C544">
-        <v>145.036</v>
+        <v>145.037</v>
       </c>
       <c r="D544">
-        <v>167.05</v>
+        <v>167.051</v>
       </c>
       <c r="E544">
         <v>147.019</v>
@@ -11307,7 +11307,7 @@
         <v>144.67</v>
       </c>
       <c r="D545">
-        <v>165.884</v>
+        <v>165.885</v>
       </c>
       <c r="E545">
         <v>144.806</v>
@@ -11324,13 +11324,13 @@
         <v>125.28</v>
       </c>
       <c r="C546">
-        <v>142.28</v>
+        <v>142.281</v>
       </c>
       <c r="D546">
         <v>164.321</v>
       </c>
       <c r="E546">
-        <v>142.199</v>
+        <v>142.2</v>
       </c>
       <c r="F546">
         <v>100</v>
@@ -11344,13 +11344,13 @@
         <v>125.089</v>
       </c>
       <c r="C547">
-        <v>141.512</v>
+        <v>141.513</v>
       </c>
       <c r="D547">
         <v>163.017</v>
       </c>
       <c r="E547">
-        <v>141.658</v>
+        <v>141.659</v>
       </c>
       <c r="F547">
         <v>100</v>
@@ -11364,13 +11364,13 @@
         <v>122.749</v>
       </c>
       <c r="C548">
-        <v>141.312</v>
+        <v>141.313</v>
       </c>
       <c r="D548">
-        <v>162.189</v>
+        <v>162.19</v>
       </c>
       <c r="E548">
-        <v>140.65</v>
+        <v>140.651</v>
       </c>
       <c r="F548">
         <v>100</v>
@@ -11387,10 +11387,10 @@
         <v>142.118</v>
       </c>
       <c r="D549">
-        <v>161.848</v>
+        <v>161.849</v>
       </c>
       <c r="E549">
-        <v>141.224</v>
+        <v>141.225</v>
       </c>
       <c r="F549">
         <v>100</v>
@@ -11404,10 +11404,10 @@
         <v>123.894</v>
       </c>
       <c r="C550">
-        <v>143.127</v>
+        <v>143.128</v>
       </c>
       <c r="D550">
-        <v>162.552</v>
+        <v>162.553</v>
       </c>
       <c r="E550">
         <v>141.973</v>
@@ -11427,7 +11427,7 @@
         <v>145.057</v>
       </c>
       <c r="D551">
-        <v>163.888</v>
+        <v>163.889</v>
       </c>
       <c r="E551">
         <v>143.2</v>
@@ -11441,16 +11441,16 @@
         <v>45405</v>
       </c>
       <c r="B552">
-        <v>122.749</v>
+        <v>122.75</v>
       </c>
       <c r="C552">
         <v>144.524</v>
       </c>
       <c r="D552">
-        <v>163.932</v>
+        <v>163.933</v>
       </c>
       <c r="E552">
-        <v>141.579</v>
+        <v>141.58</v>
       </c>
       <c r="F552">
         <v>100</v>
@@ -11461,16 +11461,16 @@
         <v>45406</v>
       </c>
       <c r="B553">
-        <v>121.287</v>
+        <v>121.288</v>
       </c>
       <c r="C553">
-        <v>142.696</v>
+        <v>142.697</v>
       </c>
       <c r="D553">
-        <v>162.675</v>
+        <v>162.676</v>
       </c>
       <c r="E553">
-        <v>141.182</v>
+        <v>141.183</v>
       </c>
       <c r="F553">
         <v>100</v>
@@ -11481,7 +11481,7 @@
         <v>45407</v>
       </c>
       <c r="B554">
-        <v>122.053</v>
+        <v>122.054</v>
       </c>
       <c r="C554">
         <v>143.06</v>
@@ -11490,7 +11490,7 @@
         <v>162.31</v>
       </c>
       <c r="E554">
-        <v>140.543</v>
+        <v>140.544</v>
       </c>
       <c r="F554">
         <v>100</v>
@@ -11501,7 +11501,7 @@
         <v>45408</v>
       </c>
       <c r="B555">
-        <v>122.163</v>
+        <v>122.164</v>
       </c>
       <c r="C555">
         <v>144.514</v>
@@ -11521,16 +11521,16 @@
         <v>45411</v>
       </c>
       <c r="B556">
-        <v>123.61</v>
+        <v>123.611</v>
       </c>
       <c r="C556">
-        <v>145.999</v>
+        <v>146</v>
       </c>
       <c r="D556">
         <v>165.458</v>
       </c>
       <c r="E556">
-        <v>142.734</v>
+        <v>142.735</v>
       </c>
       <c r="F556">
         <v>100</v>
@@ -11547,10 +11547,10 @@
         <v>147.706</v>
       </c>
       <c r="D557">
-        <v>166.764</v>
+        <v>166.765</v>
       </c>
       <c r="E557">
-        <v>143.389</v>
+        <v>143.39</v>
       </c>
       <c r="F557">
         <v>100</v>
@@ -11570,7 +11570,7 @@
         <v>168.43</v>
       </c>
       <c r="E558">
-        <v>144.923</v>
+        <v>144.924</v>
       </c>
       <c r="F558">
         <v>100</v>
@@ -11584,10 +11584,10 @@
         <v>124.606</v>
       </c>
       <c r="C559">
-        <v>150.966</v>
+        <v>150.967</v>
       </c>
       <c r="D559">
-        <v>169.8</v>
+        <v>169.801</v>
       </c>
       <c r="E559">
         <v>147.498</v>
@@ -11607,10 +11607,10 @@
         <v>152.84</v>
       </c>
       <c r="D560">
-        <v>170.283</v>
+        <v>170.284</v>
       </c>
       <c r="E560">
-        <v>150.281</v>
+        <v>150.282</v>
       </c>
       <c r="F560">
         <v>100</v>
@@ -11621,10 +11621,10 @@
         <v>45419</v>
       </c>
       <c r="B561">
-        <v>123.184</v>
+        <v>123.185</v>
       </c>
       <c r="C561">
-        <v>151.384</v>
+        <v>151.385</v>
       </c>
       <c r="D561">
         <v>170.295</v>
@@ -11644,13 +11644,13 @@
         <v>122.676</v>
       </c>
       <c r="C562">
-        <v>150.827</v>
+        <v>150.828</v>
       </c>
       <c r="D562">
-        <v>170.227</v>
+        <v>170.228</v>
       </c>
       <c r="E562">
-        <v>148.864</v>
+        <v>148.865</v>
       </c>
       <c r="F562">
         <v>100</v>
@@ -11661,13 +11661,13 @@
         <v>45421</v>
       </c>
       <c r="B563">
-        <v>121.982</v>
+        <v>121.983</v>
       </c>
       <c r="C563">
         <v>149.69</v>
       </c>
       <c r="D563">
-        <v>170.026</v>
+        <v>170.027</v>
       </c>
       <c r="E563">
         <v>149.152</v>
@@ -11681,16 +11681,16 @@
         <v>45422</v>
       </c>
       <c r="B564">
-        <v>125.255</v>
+        <v>125.256</v>
       </c>
       <c r="C564">
-        <v>149.74</v>
+        <v>149.741</v>
       </c>
       <c r="D564">
         <v>167.564</v>
       </c>
       <c r="E564">
-        <v>149.075</v>
+        <v>149.076</v>
       </c>
       <c r="F564">
         <v>100</v>
@@ -11701,13 +11701,13 @@
         <v>45425</v>
       </c>
       <c r="B565">
-        <v>123.61</v>
+        <v>123.611</v>
       </c>
       <c r="C565">
-        <v>149.2</v>
+        <v>149.201</v>
       </c>
       <c r="D565">
-        <v>167.274</v>
+        <v>167.275</v>
       </c>
       <c r="E565">
         <v>146.639</v>
@@ -11721,16 +11721,16 @@
         <v>45426</v>
       </c>
       <c r="B566">
-        <v>121.817</v>
+        <v>121.818</v>
       </c>
       <c r="C566">
-        <v>148.914</v>
+        <v>148.915</v>
       </c>
       <c r="D566">
-        <v>166.463</v>
+        <v>166.464</v>
       </c>
       <c r="E566">
-        <v>145.989</v>
+        <v>145.99</v>
       </c>
       <c r="F566">
         <v>100</v>
@@ -11741,13 +11741,13 @@
         <v>45427</v>
       </c>
       <c r="B567">
-        <v>121.972</v>
+        <v>121.973</v>
       </c>
       <c r="C567">
         <v>149.03</v>
       </c>
       <c r="D567">
-        <v>166.507</v>
+        <v>166.508</v>
       </c>
       <c r="E567">
         <v>145.639</v>
@@ -11767,10 +11767,10 @@
         <v>149.161</v>
       </c>
       <c r="D568">
-        <v>166.183</v>
+        <v>166.184</v>
       </c>
       <c r="E568">
-        <v>145.412</v>
+        <v>145.413</v>
       </c>
       <c r="F568">
         <v>100</v>
@@ -11781,16 +11781,16 @@
         <v>45429</v>
       </c>
       <c r="B569">
-        <v>122.589</v>
+        <v>123.206</v>
       </c>
       <c r="C569">
-        <v>147.09</v>
+        <v>147.83</v>
       </c>
       <c r="D569">
-        <v>164.842</v>
+        <v>165.672</v>
       </c>
       <c r="E569">
-        <v>143.687</v>
+        <v>144.41</v>
       </c>
       <c r="F569">
         <v>100</v>
@@ -11804,10 +11804,10 @@
         <v>121.33</v>
       </c>
       <c r="C570">
-        <v>146.111</v>
+        <v>146.112</v>
       </c>
       <c r="D570">
-        <v>163.492</v>
+        <v>163.493</v>
       </c>
       <c r="E570">
         <v>142.509</v>
@@ -11827,7 +11827,7 @@
         <v>144.913</v>
       </c>
       <c r="D571">
-        <v>162.377</v>
+        <v>162.378</v>
       </c>
       <c r="E571">
         <v>140.033</v>
@@ -11841,13 +11841,13 @@
         <v>45434</v>
       </c>
       <c r="B572">
-        <v>120.955</v>
+        <v>120.956</v>
       </c>
       <c r="C572">
-        <v>142.358</v>
+        <v>142.359</v>
       </c>
       <c r="D572">
-        <v>159.278</v>
+        <v>159.279</v>
       </c>
       <c r="E572">
         <v>137.425</v>
@@ -11861,7 +11861,7 @@
         <v>45435</v>
       </c>
       <c r="B573">
-        <v>119.606</v>
+        <v>119.607</v>
       </c>
       <c r="C573">
         <v>140.296</v>
@@ -11887,10 +11887,10 @@
         <v>143.612</v>
       </c>
       <c r="D574">
-        <v>160.073</v>
+        <v>160.074</v>
       </c>
       <c r="E574">
-        <v>137.496</v>
+        <v>137.497</v>
       </c>
       <c r="F574">
         <v>100</v>
@@ -11901,16 +11901,16 @@
         <v>45439</v>
       </c>
       <c r="B575">
-        <v>122.729</v>
+        <v>122.73</v>
       </c>
       <c r="C575">
         <v>145.374</v>
       </c>
       <c r="D575">
-        <v>162.492</v>
+        <v>162.493</v>
       </c>
       <c r="E575">
-        <v>139.332</v>
+        <v>139.333</v>
       </c>
       <c r="F575">
         <v>100</v>
@@ -11921,16 +11921,16 @@
         <v>45440</v>
       </c>
       <c r="B576">
-        <v>122.528</v>
+        <v>122.529</v>
       </c>
       <c r="C576">
-        <v>144.928</v>
+        <v>144.929</v>
       </c>
       <c r="D576">
-        <v>162.628</v>
+        <v>162.629</v>
       </c>
       <c r="E576">
-        <v>140.688</v>
+        <v>140.689</v>
       </c>
       <c r="F576">
         <v>100</v>
@@ -11941,16 +11941,16 @@
         <v>45441</v>
       </c>
       <c r="B577">
-        <v>120.818</v>
+        <v>120.819</v>
       </c>
       <c r="C577">
-        <v>144.588</v>
+        <v>144.589</v>
       </c>
       <c r="D577">
         <v>161.177</v>
       </c>
       <c r="E577">
-        <v>140.847</v>
+        <v>140.848</v>
       </c>
       <c r="F577">
         <v>100</v>
@@ -11964,13 +11964,13 @@
         <v>121.122</v>
       </c>
       <c r="C578">
-        <v>145.908</v>
+        <v>145.909</v>
       </c>
       <c r="D578">
-        <v>163.663</v>
+        <v>163.664</v>
       </c>
       <c r="E578">
-        <v>141.665</v>
+        <v>141.666</v>
       </c>
       <c r="F578">
         <v>100</v>
@@ -11984,13 +11984,13 @@
         <v>121.37</v>
       </c>
       <c r="C579">
-        <v>146.421</v>
+        <v>146.422</v>
       </c>
       <c r="D579">
         <v>163.665</v>
       </c>
       <c r="E579">
-        <v>141.024</v>
+        <v>141.025</v>
       </c>
       <c r="F579">
         <v>100</v>
@@ -12010,7 +12010,7 @@
         <v>162.472</v>
       </c>
       <c r="E580">
-        <v>141.222</v>
+        <v>141.223</v>
       </c>
       <c r="F580">
         <v>100</v>
@@ -12024,7 +12024,7 @@
         <v>118.662</v>
       </c>
       <c r="C581">
-        <v>144.361</v>
+        <v>144.362</v>
       </c>
       <c r="D581">
         <v>158.846</v>
@@ -15615,10 +15615,10 @@
         <v>45049</v>
       </c>
       <c r="B325">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C325">
-        <v>0.638</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="326" spans="1:3">
@@ -15629,7 +15629,7 @@
         <v>469</v>
       </c>
       <c r="C326">
-        <v>-0.638</v>
+        <v>-1.06</v>
       </c>
     </row>
     <row r="327" spans="1:3">
@@ -17903,10 +17903,10 @@
         <v>45363</v>
       </c>
       <c r="B533">
-        <v>1020</v>
+        <v>1005</v>
       </c>
       <c r="C533">
-        <v>2.482</v>
+        <v>1</v>
       </c>
     </row>
     <row r="534" spans="1:3">
@@ -17917,7 +17917,7 @@
         <v>1035</v>
       </c>
       <c r="C534">
-        <v>1.46</v>
+        <v>2.941</v>
       </c>
     </row>
     <row r="535" spans="1:3">
@@ -17947,10 +17947,10 @@
         <v>45369</v>
       </c>
       <c r="B537">
-        <v>1025</v>
+        <v>1015</v>
       </c>
       <c r="C537">
-        <v>0</v>
+        <v>-0.98</v>
       </c>
     </row>
     <row r="538" spans="1:3">
@@ -17961,7 +17961,7 @@
         <v>1025</v>
       </c>
       <c r="C538">
-        <v>0</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="539" spans="1:3">
@@ -18376,10 +18376,10 @@
         <v>45429</v>
       </c>
       <c r="B576">
-        <v>1120</v>
+        <v>1105</v>
       </c>
       <c r="C576">
-        <v>1.802</v>
+        <v>0.454</v>
       </c>
     </row>
     <row r="577" spans="1:3">
@@ -18390,7 +18390,7 @@
         <v>1180</v>
       </c>
       <c r="C577">
-        <v>5.219</v>
+        <v>6.567</v>
       </c>
     </row>
     <row r="578" spans="1:3">

</xml_diff>